<commit_message>
Fixed grammar and style
</commit_message>
<xml_diff>
--- a/Evaluation/CQs-query-output.xlsx
+++ b/Evaluation/CQs-query-output.xlsx
@@ -2292,8 +2292,8 @@
   </sheetPr>
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2336,7 +2336,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="1256.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="1132.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="235.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="1141.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="1143.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="302.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="303.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -2380,7 +2380,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="559.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="561.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="447.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="449.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="514.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="516.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="537.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="538.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
         <v>30</v>
       </c>

</xml_diff>